<commit_message>
data helper clas has beeen modified
</commit_message>
<xml_diff>
--- a/DataDrivenPOIArtifactID/src/test/java/utility/TestCase.xlsx
+++ b/DataDrivenPOIArtifactID/src/test/java/utility/TestCase.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="70">
   <si>
     <t xml:space="preserve">UserName</t>
   </si>
@@ -30,15 +30,24 @@
     <t xml:space="preserve">Password</t>
   </si>
   <si>
+    <t xml:space="preserve">login</t>
+  </si>
+  <si>
     <t xml:space="preserve">a</t>
   </si>
   <si>
+    <t xml:space="preserve">success</t>
+  </si>
+  <si>
     <t xml:space="preserve">b</t>
   </si>
   <si>
     <t xml:space="preserve">alex</t>
   </si>
   <si>
+    <t xml:space="preserve">fail</t>
+  </si>
+  <si>
     <t xml:space="preserve">d</t>
   </si>
   <si>
@@ -60,9 +69,6 @@
     <t xml:space="preserve">lusy</t>
   </si>
   <si>
-    <t xml:space="preserve">hareg</t>
-  </si>
-  <si>
     <t xml:space="preserve">salima</t>
   </si>
   <si>
@@ -109,9 +115,6 @@
   </si>
   <si>
     <t xml:space="preserve">Click</t>
-  </si>
-  <si>
-    <t xml:space="preserve">login</t>
   </si>
   <si>
     <t xml:space="preserve">Test yahoo search box is working or not</t>
@@ -454,10 +457,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -472,85 +475,117 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>9</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="0" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -577,8 +612,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.67"/>
@@ -586,29 +621,29 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -618,63 +653,63 @@
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5"/>
       <c r="B4" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5"/>
       <c r="B5" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5"/>
       <c r="B6" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5"/>
       <c r="B7" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -684,34 +719,34 @@
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5"/>
       <c r="B9" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5"/>
       <c r="B10" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -721,78 +756,78 @@
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5"/>
       <c r="B12" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5"/>
       <c r="B13" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5"/>
       <c r="B14" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5"/>
       <c r="B15" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5"/>
       <c r="B16" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -802,63 +837,63 @@
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5"/>
       <c r="B18" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5"/>
       <c r="B19" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5"/>
       <c r="B20" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5"/>
       <c r="B21" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -868,63 +903,63 @@
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5"/>
       <c r="B23" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5"/>
       <c r="B24" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5"/>
       <c r="B25" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5"/>
       <c r="B26" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -934,43 +969,43 @@
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5"/>
       <c r="B28" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5"/>
       <c r="B29" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5"/>
       <c r="B30" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E30" s="7"/>
     </row>
@@ -1009,90 +1044,90 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>